<commit_message>
Add all necessary questions to the diagnosis form
</commit_message>
<xml_diff>
--- a/data/hobby_options.xlsx
+++ b/data/hobby_options.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\伊藤駿\Desktop\適職診断サイト作成\ウェブサイト構築\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_tekishokusindanwebsite\website\myapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16C501FE-EC34-459A-BC3B-A626762984A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3225C55D-C297-428F-98AD-73A6E699494A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{2606A51F-AD8F-4958-8098-FD6CD9172424}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{2606A51F-AD8F-4958-8098-FD6CD9172424}"/>
   </bookViews>
   <sheets>
     <sheet name="趣味リスト" sheetId="1" r:id="rId1"/>
@@ -34,11 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="2"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>趣味</t>
     <rPh sb="0" eb="2">
@@ -510,264 +506,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B460C744-502C-41B4-B0F5-B35F34734355}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.625" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>